<commit_message>
Data files for March release updated + 2024 post ops.
</commit_message>
<xml_diff>
--- a/static/download/2024/RP3_APT_ASMA_2024_Jan_Dec.xlsx
+++ b/static/download/2024/RP3_APT_ASMA_2024_Jan_Dec.xlsx
@@ -753,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="9">
-        <v>45729.0</v>
+        <v>45758.0</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
@@ -836,11 +836,10 @@
         <v>94241.0</v>
       </c>
       <c r="E6" s="28">
-        <f t="shared" ref="E6:E17" si="1">F6/D6</f>
-        <v>0.7296671123</v>
+        <v>0.73</v>
       </c>
       <c r="F6" s="27">
-        <v>68764.55833</v>
+        <v>68765.0</v>
       </c>
       <c r="G6" s="29">
         <v>12.67</v>
@@ -860,11 +859,10 @@
         <v>92129.0</v>
       </c>
       <c r="E7" s="28">
-        <f t="shared" si="1"/>
-        <v>0.8143249321</v>
+        <v>0.81</v>
       </c>
       <c r="F7" s="27">
-        <v>75022.94167</v>
+        <v>75023.0</v>
       </c>
       <c r="G7" s="28">
         <v>13.24</v>
@@ -884,11 +882,10 @@
         <v>214165.0</v>
       </c>
       <c r="E8" s="28">
-        <f t="shared" si="1"/>
-        <v>1.484292213</v>
+        <v>1.48</v>
       </c>
       <c r="F8" s="27">
-        <v>317883.4417</v>
+        <v>317883.0</v>
       </c>
       <c r="G8" s="29">
         <v>14.01</v>
@@ -908,11 +905,10 @@
         <v>57786.0</v>
       </c>
       <c r="E9" s="28">
-        <f t="shared" si="1"/>
-        <v>0.8234514704</v>
+        <v>0.82</v>
       </c>
       <c r="F9" s="27">
-        <v>47583.96667</v>
+        <v>47584.0</v>
       </c>
       <c r="G9" s="28">
         <v>13.75</v>
@@ -932,11 +928,10 @@
         <v>52210.0</v>
       </c>
       <c r="E10" s="28">
-        <f t="shared" si="1"/>
-        <v>1.255147481</v>
+        <v>1.26</v>
       </c>
       <c r="F10" s="27">
-        <v>65531.25</v>
+        <v>65531.0</v>
       </c>
       <c r="G10" s="29">
         <v>13.58</v>
@@ -956,11 +951,10 @@
         <v>75453.0</v>
       </c>
       <c r="E11" s="28">
-        <f t="shared" si="1"/>
-        <v>0.8667145994</v>
+        <v>0.87</v>
       </c>
       <c r="F11" s="27">
-        <v>65396.21667</v>
+        <v>65396.0</v>
       </c>
       <c r="G11" s="29">
         <v>13.11</v>
@@ -980,11 +974,10 @@
         <v>158091.0</v>
       </c>
       <c r="E12" s="28">
-        <f t="shared" si="1"/>
-        <v>1.202817154</v>
+        <v>1.2</v>
       </c>
       <c r="F12" s="27">
-        <v>190154.5667</v>
+        <v>190155.0</v>
       </c>
       <c r="G12" s="29">
         <v>12.82</v>
@@ -1004,11 +997,10 @@
         <v>39550.0</v>
       </c>
       <c r="E13" s="28">
-        <f t="shared" si="1"/>
-        <v>0.4546188369</v>
+        <v>0.45</v>
       </c>
       <c r="F13" s="27">
-        <v>17980.175</v>
+        <v>17980.0</v>
       </c>
       <c r="G13" s="29">
         <v>12.88</v>
@@ -1028,11 +1020,10 @@
         <v>71170.0</v>
       </c>
       <c r="E14" s="28">
-        <f t="shared" si="1"/>
-        <v>0.9482932883</v>
+        <v>0.95</v>
       </c>
       <c r="F14" s="27">
-        <v>67490.03333</v>
+        <v>67490.0</v>
       </c>
       <c r="G14" s="29">
         <v>12.02</v>
@@ -1052,11 +1043,10 @@
         <v>238241.0</v>
       </c>
       <c r="E15" s="28">
-        <f t="shared" si="1"/>
-        <v>1.234454852</v>
+        <v>1.23</v>
       </c>
       <c r="F15" s="27">
-        <v>294097.7583</v>
+        <v>294098.0</v>
       </c>
       <c r="G15" s="28">
         <v>13.26</v>
@@ -1076,11 +1066,10 @@
         <v>118523.0</v>
       </c>
       <c r="E16" s="28">
-        <f t="shared" si="1"/>
-        <v>1.67831314</v>
+        <v>1.68</v>
       </c>
       <c r="F16" s="27">
-        <v>198918.7083</v>
+        <v>198919.0</v>
       </c>
       <c r="G16" s="29">
         <v>12.65</v>
@@ -1100,11 +1089,10 @@
         <v>115214.0</v>
       </c>
       <c r="E17" s="28">
-        <f t="shared" si="1"/>
-        <v>0.9608851789</v>
+        <v>0.96</v>
       </c>
       <c r="F17" s="27">
-        <v>110707.425</v>
+        <v>110707.0</v>
       </c>
       <c r="G17" s="28">
         <v>13.01</v>
@@ -1139,11 +1127,10 @@
         <v>105900.0</v>
       </c>
       <c r="E19" s="28">
-        <f t="shared" ref="E19:E47" si="2">F19/D19</f>
-        <v>1.008329478</v>
+        <v>1.01</v>
       </c>
       <c r="F19" s="27">
-        <v>106782.0917</v>
+        <v>106782.0</v>
       </c>
       <c r="G19" s="28">
         <v>12.66</v>
@@ -1163,11 +1150,10 @@
         <v>88721.0</v>
       </c>
       <c r="E20" s="28">
-        <f t="shared" si="2"/>
-        <v>1.334593933</v>
+        <v>1.33</v>
       </c>
       <c r="F20" s="27">
-        <v>118406.5083</v>
+        <v>118407.0</v>
       </c>
       <c r="G20" s="29">
         <v>12.54</v>
@@ -1187,11 +1173,10 @@
         <v>93125.0</v>
       </c>
       <c r="E21" s="28">
-        <f t="shared" si="2"/>
-        <v>0.7492642505</v>
+        <v>0.75</v>
       </c>
       <c r="F21" s="27">
-        <v>69775.23333</v>
+        <v>69775.0</v>
       </c>
       <c r="G21" s="29">
         <v>12.65</v>
@@ -1211,11 +1196,10 @@
         <v>54804.0</v>
       </c>
       <c r="E22" s="28">
-        <f t="shared" si="2"/>
-        <v>1.742471048</v>
+        <v>1.74</v>
       </c>
       <c r="F22" s="27">
-        <v>95494.38333</v>
+        <v>95494.0</v>
       </c>
       <c r="G22" s="28">
         <v>14.93</v>
@@ -1235,11 +1219,10 @@
         <v>57019.0</v>
       </c>
       <c r="E23" s="28">
-        <f t="shared" si="2"/>
-        <v>0.9717599981</v>
+        <v>0.97</v>
       </c>
       <c r="F23" s="27">
-        <v>55408.78333</v>
+        <v>55409.0</v>
       </c>
       <c r="G23" s="28">
         <v>13.84</v>
@@ -1259,11 +1242,10 @@
         <v>166842.0</v>
       </c>
       <c r="E24" s="28">
-        <f t="shared" si="2"/>
-        <v>2.328931314</v>
+        <v>2.33</v>
       </c>
       <c r="F24" s="27">
-        <v>388563.5583</v>
+        <v>388564.0</v>
       </c>
       <c r="G24" s="28">
         <v>12.9</v>
@@ -1283,11 +1265,10 @@
         <v>200923.0</v>
       </c>
       <c r="E25" s="28">
-        <f t="shared" si="2"/>
-        <v>1.089579258</v>
+        <v>1.09</v>
       </c>
       <c r="F25" s="27">
-        <v>218921.5333</v>
+        <v>218922.0</v>
       </c>
       <c r="G25" s="28">
         <v>12.83</v>
@@ -1307,11 +1288,10 @@
         <v>81103.0</v>
       </c>
       <c r="E26" s="28">
-        <f t="shared" si="2"/>
-        <v>1.621480401</v>
+        <v>1.62</v>
       </c>
       <c r="F26" s="27">
-        <v>131506.925</v>
+        <v>131507.0</v>
       </c>
       <c r="G26" s="29">
         <v>13.77</v>
@@ -1331,11 +1311,10 @@
         <v>108017.0</v>
       </c>
       <c r="E27" s="28">
-        <f t="shared" si="2"/>
-        <v>1.355149035</v>
+        <v>1.36</v>
       </c>
       <c r="F27" s="27">
-        <v>146379.1333</v>
+        <v>146379.0</v>
       </c>
       <c r="G27" s="29">
         <v>12.87</v>
@@ -1355,11 +1334,10 @@
         <v>32849.0</v>
       </c>
       <c r="E28" s="28">
-        <f t="shared" si="2"/>
-        <v>0.5108547192</v>
+        <v>0.51</v>
       </c>
       <c r="F28" s="27">
-        <v>16781.06667</v>
+        <v>16781.0</v>
       </c>
       <c r="G28" s="28">
         <v>13.22</v>
@@ -1379,11 +1357,10 @@
         <v>44231.0</v>
       </c>
       <c r="E29" s="28">
-        <f t="shared" si="2"/>
-        <v>0.4475767374</v>
+        <v>0.45</v>
       </c>
       <c r="F29" s="27">
-        <v>19796.76667</v>
+        <v>19797.0</v>
       </c>
       <c r="G29" s="28">
         <v>12.51</v>
@@ -1403,11 +1380,10 @@
         <v>47585.0</v>
       </c>
       <c r="E30" s="28">
-        <f t="shared" si="2"/>
-        <v>0.6687632657</v>
+        <v>0.67</v>
       </c>
       <c r="F30" s="27">
-        <v>31823.1</v>
+        <v>31823.0</v>
       </c>
       <c r="G30" s="29">
         <v>11.97</v>
@@ -1427,11 +1403,10 @@
         <v>72502.0</v>
       </c>
       <c r="E31" s="28">
-        <f t="shared" si="2"/>
-        <v>1.462643214</v>
+        <v>1.46</v>
       </c>
       <c r="F31" s="27">
-        <v>106044.5583</v>
+        <v>106045.0</v>
       </c>
       <c r="G31" s="28">
         <v>14.1</v>
@@ -1451,11 +1426,10 @@
         <v>224869.0</v>
       </c>
       <c r="E32" s="28">
-        <f t="shared" si="2"/>
-        <v>0.9745876488</v>
+        <v>0.97</v>
       </c>
       <c r="F32" s="27">
-        <v>219154.55</v>
+        <v>219155.0</v>
       </c>
       <c r="G32" s="29">
         <v>14.43</v>
@@ -1475,11 +1449,10 @@
         <v>101402.0</v>
       </c>
       <c r="E33" s="28">
-        <f t="shared" si="2"/>
-        <v>0.962486851</v>
+        <v>0.96</v>
       </c>
       <c r="F33" s="27">
-        <v>97598.09167</v>
+        <v>97598.0</v>
       </c>
       <c r="G33" s="28">
         <v>13.91</v>
@@ -1499,11 +1472,10 @@
         <v>117254.0</v>
       </c>
       <c r="E34" s="28">
-        <f t="shared" si="2"/>
-        <v>1.548014283</v>
+        <v>1.55</v>
       </c>
       <c r="F34" s="27">
-        <v>181510.8667</v>
+        <v>181511.0</v>
       </c>
       <c r="G34" s="29">
         <v>13.08</v>
@@ -1523,11 +1495,10 @@
         <v>60462.0</v>
       </c>
       <c r="E35" s="28">
-        <f t="shared" si="2"/>
-        <v>0.7706559492</v>
+        <v>0.77</v>
       </c>
       <c r="F35" s="27">
-        <v>46595.4</v>
+        <v>46595.0</v>
       </c>
       <c r="G35" s="29">
         <v>13.38</v>
@@ -1547,11 +1518,10 @@
         <v>104873.0</v>
       </c>
       <c r="E36" s="28">
-        <f t="shared" si="2"/>
-        <v>2.173611972</v>
+        <v>2.17</v>
       </c>
       <c r="F36" s="27">
-        <v>227953.2083</v>
+        <v>227953.0</v>
       </c>
       <c r="G36" s="29">
         <v>12.63</v>
@@ -1571,11 +1541,10 @@
         <v>53058.0</v>
       </c>
       <c r="E37" s="28">
-        <f t="shared" si="2"/>
-        <v>1.351833371</v>
+        <v>1.35</v>
       </c>
       <c r="F37" s="27">
-        <v>71725.575</v>
+        <v>71726.0</v>
       </c>
       <c r="G37" s="28">
         <v>13.24</v>
@@ -1595,11 +1564,10 @@
         <v>56282.0</v>
       </c>
       <c r="E38" s="28">
-        <f t="shared" si="2"/>
-        <v>1.067139731</v>
+        <v>1.07</v>
       </c>
       <c r="F38" s="27">
-        <v>60060.75833</v>
+        <v>60061.0</v>
       </c>
       <c r="G38" s="28">
         <v>11.83</v>
@@ -1619,11 +1587,10 @@
         <v>43305.0</v>
       </c>
       <c r="E39" s="28">
-        <f t="shared" si="2"/>
-        <v>1.438939307</v>
+        <v>1.44</v>
       </c>
       <c r="F39" s="27">
-        <v>62313.26667</v>
+        <v>62313.0</v>
       </c>
       <c r="G39" s="28">
         <v>11.68</v>
@@ -1643,11 +1610,10 @@
         <v>155414.0</v>
       </c>
       <c r="E40" s="28">
-        <f t="shared" si="2"/>
-        <v>1.797708808</v>
+        <v>1.8</v>
       </c>
       <c r="F40" s="27">
-        <v>279389.1167</v>
+        <v>279389.0</v>
       </c>
       <c r="G40" s="28">
         <v>12.37</v>
@@ -1667,11 +1633,10 @@
         <v>63043.0</v>
       </c>
       <c r="E41" s="28">
-        <f t="shared" si="2"/>
-        <v>0.9348534599</v>
+        <v>0.93</v>
       </c>
       <c r="F41" s="27">
-        <v>58935.96667</v>
+        <v>58936.0</v>
       </c>
       <c r="G41" s="29">
         <v>12.78</v>
@@ -1691,11 +1656,10 @@
         <v>120604.0</v>
       </c>
       <c r="E42" s="28">
-        <f t="shared" si="2"/>
-        <v>1.172101119</v>
+        <v>1.17</v>
       </c>
       <c r="F42" s="27">
-        <v>141360.0833</v>
+        <v>141360.0</v>
       </c>
       <c r="G42" s="29">
         <v>12.56</v>
@@ -1715,11 +1679,10 @@
         <v>52100.0</v>
       </c>
       <c r="E43" s="28">
-        <f t="shared" si="2"/>
-        <v>1.174122201</v>
+        <v>1.17</v>
       </c>
       <c r="F43" s="27">
-        <v>61171.76667</v>
+        <v>61172.0</v>
       </c>
       <c r="G43" s="29">
         <v>13.48</v>
@@ -1739,11 +1702,10 @@
         <v>112588.0</v>
       </c>
       <c r="E44" s="28">
-        <f t="shared" si="2"/>
-        <v>3.170132918</v>
+        <v>3.17</v>
       </c>
       <c r="F44" s="27">
-        <v>356918.925</v>
+        <v>356919.0</v>
       </c>
       <c r="G44" s="28">
         <v>14.07</v>
@@ -1763,11 +1725,10 @@
         <v>57002.0</v>
       </c>
       <c r="E45" s="28">
-        <f t="shared" si="2"/>
-        <v>0.6590099177</v>
+        <v>0.66</v>
       </c>
       <c r="F45" s="27">
-        <v>37564.88333</v>
+        <v>37565.0</v>
       </c>
       <c r="G45" s="28">
         <v>12.08</v>
@@ -1787,11 +1748,10 @@
         <v>84390.0</v>
       </c>
       <c r="E46" s="28">
-        <f t="shared" si="2"/>
-        <v>1.551604653</v>
+        <v>1.55</v>
       </c>
       <c r="F46" s="27">
-        <v>130939.9167</v>
+        <v>130940.0</v>
       </c>
       <c r="G46" s="29">
         <v>13.67</v>
@@ -1811,11 +1771,10 @@
         <v>123593.0</v>
       </c>
       <c r="E47" s="28">
-        <f t="shared" si="2"/>
-        <v>2.332490513</v>
+        <v>2.33</v>
       </c>
       <c r="F47" s="27">
-        <v>288279.5</v>
+        <v>288280.0</v>
       </c>
       <c r="G47" s="28">
         <v>13.36</v>

</xml_diff>